<commit_message>
Versões em 1080p e 720p regeradas a partir dos arquivos 1440p em .xcf. / Parâmetros para 1080p e 720p redefinidos. / Obtidos dados das variações em 1080p com RPI4
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="64">
   <si>
     <t>Scene</t>
   </si>
@@ -102,6 +102,12 @@
     <t>160 minus</t>
   </si>
   <si>
+    <t>Min. Size Face: 1.0 / Scale Factor: 1.039 / Min. Neighbors: 3</t>
+  </si>
+  <si>
+    <t>1080 x 1920</t>
+  </si>
+  <si>
     <t>Metric</t>
   </si>
   <si>
@@ -141,6 +147,21 @@
     <t>84,144 / 0.8%</t>
   </si>
   <si>
+    <t>304,770 / 4.9%</t>
+  </si>
+  <si>
+    <t>238,938 / 3.8%</t>
+  </si>
+  <si>
+    <t>186,732 / 3.0%</t>
+  </si>
+  <si>
+    <t>127,410 / 2.0%</t>
+  </si>
+  <si>
+    <t>83,460 / 1.3%</t>
+  </si>
+  <si>
     <t>1.6 - Encoded Faces Images Total Size (bytes) / (% from full image encoded size)</t>
   </si>
   <si>
@@ -157,6 +178,21 @@
   </si>
   <si>
     <t>115,868 / 0.8%</t>
+  </si>
+  <si>
+    <t>424,700 / 5.1%</t>
+  </si>
+  <si>
+    <t>332,764 / 4.0%</t>
+  </si>
+  <si>
+    <t>259,464 / 3.1%</t>
+  </si>
+  <si>
+    <t>175,964 / 2.1%</t>
+  </si>
+  <si>
+    <t>114,540 / 1.4%</t>
   </si>
   <si>
     <t>2.1 - Loading Image (s)</t>
@@ -180,11 +216,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="#,##0.000"/>
-    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="178" formatCode="#,##0.000"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -222,13 +258,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -236,7 +265,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,16 +279,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -273,6 +295,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -280,16 +325,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,24 +341,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -335,34 +387,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -391,187 +427,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -624,6 +660,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -641,9 +686,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -663,32 +740,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -697,154 +748,139 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
@@ -854,7 +890,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -870,6 +906,18 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -882,7 +930,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -891,7 +939,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1290,7 +1338,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9037037037037" defaultRowHeight="15"/>
@@ -1311,895 +1359,1027 @@
     <col min="19" max="19" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="1" ht="75" spans="1:19">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="9" customFormat="1" ht="75" spans="1:19">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="13">
         <v>11059200</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="14">
         <v>14745672</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="11">
         <v>169</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="15">
         <v>539058</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="15">
         <v>742472</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="11">
         <v>0.312</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="11">
         <v>0.007</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="11">
         <v>3.293</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="11">
         <v>0.011</v>
       </c>
-      <c r="O2" s="12">
+      <c r="O2" s="16">
         <v>3.623</v>
       </c>
-      <c r="P2" s="13">
+      <c r="P2" s="17">
         <f>1/O2</f>
         <v>0.276014352746343</v>
       </c>
-      <c r="Q2" s="13">
+      <c r="Q2" s="17">
         <f>G2*P2/1000000</f>
         <v>4.07001711288987</v>
       </c>
-      <c r="R2" s="13">
+      <c r="R2" s="17">
         <f>J2*P2/1000000</f>
         <v>0.204932928512283</v>
       </c>
-      <c r="S2" s="14">
+      <c r="S2" s="18">
         <f>R2/Q2</f>
         <v>0.0503518591760348</v>
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="13">
         <v>11059200</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="14">
         <v>14745672</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="11">
         <v>130</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="15">
         <v>408060</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="15">
         <v>562352</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="11">
         <v>0.309</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="11">
         <v>0.007</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="11">
         <v>3.286</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="11">
         <v>0.009</v>
       </c>
-      <c r="O3" s="12">
+      <c r="O3" s="16">
         <v>3.611</v>
       </c>
-      <c r="P3" s="13">
+      <c r="P3" s="17">
         <f t="shared" ref="P3:P21" si="0">1/O3</f>
         <v>0.27693159789532</v>
       </c>
-      <c r="Q3" s="13">
+      <c r="Q3" s="17">
         <f t="shared" ref="Q3:Q21" si="1">G3*P3/1000000</f>
         <v>4.08354250900028</v>
       </c>
-      <c r="R3" s="13">
+      <c r="R3" s="17">
         <f t="shared" ref="R3:R21" si="2">J3*P3/1000000</f>
         <v>0.155733037939629</v>
       </c>
-      <c r="S3" s="14">
+      <c r="S3" s="18">
         <f t="shared" ref="S3:S21" si="3">R3/Q3</f>
         <v>0.0381367495492915</v>
       </c>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="13">
         <v>11059200</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="14">
         <v>14745672</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="11">
         <v>95</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="15">
         <v>289590</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="15">
         <v>399528</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="11">
         <v>0.309</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="11">
         <v>0.007</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="11">
         <v>3.272</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="11">
         <v>0.006</v>
       </c>
-      <c r="O4" s="12">
+      <c r="O4" s="16">
         <v>3.594</v>
       </c>
-      <c r="P4" s="13">
+      <c r="P4" s="17">
         <f t="shared" si="0"/>
         <v>0.278241513633834</v>
       </c>
-      <c r="Q4" s="13">
+      <c r="Q4" s="17">
         <f t="shared" si="1"/>
         <v>4.10285809682805</v>
       </c>
-      <c r="R4" s="13">
+      <c r="R4" s="17">
         <f t="shared" si="2"/>
         <v>0.111165275459099</v>
       </c>
-      <c r="S4" s="14">
+      <c r="S4" s="18">
         <f t="shared" si="3"/>
         <v>0.0270945942646764</v>
       </c>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="13">
         <v>11059200</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="14">
         <v>14745672</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="11">
         <v>58</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="15">
         <v>174954</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="15">
         <v>241748</v>
       </c>
-      <c r="K5" s="7">
+      <c r="K5" s="11">
         <v>0.301</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5" s="11">
         <v>0.007</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="11">
         <v>3.218</v>
       </c>
-      <c r="N5" s="7">
+      <c r="N5" s="11">
         <v>0.003</v>
       </c>
-      <c r="O5" s="12">
+      <c r="O5" s="16">
         <v>3.529</v>
       </c>
-      <c r="P5" s="13">
+      <c r="P5" s="17">
         <f t="shared" si="0"/>
         <v>0.28336639274582</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="17">
         <f t="shared" si="1"/>
         <v>4.17842788325305</v>
       </c>
-      <c r="R5" s="13">
+      <c r="R5" s="17">
         <f t="shared" si="2"/>
         <v>0.0685032587135166</v>
       </c>
-      <c r="S5" s="14">
+      <c r="S5" s="18">
         <f t="shared" si="3"/>
         <v>0.0163945054521761</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="13">
         <v>11059200</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="14">
         <v>14745672</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="11">
         <v>25</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="15">
         <v>84144</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="15">
         <v>115868</v>
       </c>
-      <c r="K6" s="7">
+      <c r="K6" s="11">
         <v>0.299</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6" s="11">
         <v>0.007</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="11">
         <v>3.178</v>
       </c>
-      <c r="N6" s="7">
+      <c r="N6" s="11">
         <v>0.002</v>
       </c>
-      <c r="O6" s="12">
+      <c r="O6" s="16">
         <v>3.486</v>
       </c>
-      <c r="P6" s="13">
+      <c r="P6" s="17">
         <f t="shared" si="0"/>
         <v>0.286861732644865</v>
       </c>
-      <c r="Q6" s="13">
+      <c r="Q6" s="17">
         <f t="shared" si="1"/>
         <v>4.22996901893287</v>
       </c>
-      <c r="R6" s="13">
+      <c r="R6" s="17">
         <f t="shared" si="2"/>
         <v>0.0332380952380952</v>
       </c>
-      <c r="S6" s="14">
+      <c r="S6" s="18">
         <f t="shared" si="3"/>
         <v>0.00785776328132078</v>
       </c>
     </row>
     <row r="7" spans="1:19">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="7" t="s">
+      <c r="B7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="13" t="e">
+      <c r="D7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="13">
+        <v>6220800</v>
+      </c>
+      <c r="G7" s="14">
+        <v>8294472</v>
+      </c>
+      <c r="H7" s="11">
+        <v>146</v>
+      </c>
+      <c r="I7" s="15">
+        <v>304770</v>
+      </c>
+      <c r="J7" s="15">
+        <v>424700</v>
+      </c>
+      <c r="K7" s="11">
+        <v>0.274</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.004</v>
+      </c>
+      <c r="M7" s="11">
+        <v>3.27</v>
+      </c>
+      <c r="N7" s="11">
+        <v>0.007</v>
+      </c>
+      <c r="O7" s="16">
+        <v>3.555</v>
+      </c>
+      <c r="P7" s="17">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q7" s="13" t="e">
+        <v>0.281293952180028</v>
+      </c>
+      <c r="Q7" s="17">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R7" s="13" t="e">
+        <v>2.33318481012658</v>
+      </c>
+      <c r="R7" s="17">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" s="14" t="e">
+        <v>0.119465541490858</v>
+      </c>
+      <c r="S7" s="18">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.0512027769820671</v>
       </c>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="7" t="s">
+      <c r="B8" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="13" t="e">
+      <c r="D8" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="13">
+        <v>6220800</v>
+      </c>
+      <c r="G8" s="14">
+        <v>8294472</v>
+      </c>
+      <c r="H8" s="11">
+        <v>113</v>
+      </c>
+      <c r="I8" s="15">
+        <v>238938</v>
+      </c>
+      <c r="J8" s="15">
+        <v>332764</v>
+      </c>
+      <c r="K8" s="11">
+        <v>0.267</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.004</v>
+      </c>
+      <c r="M8" s="11">
+        <v>3.202</v>
+      </c>
+      <c r="N8" s="11">
+        <v>0.006</v>
+      </c>
+      <c r="O8" s="16">
+        <v>3.479</v>
+      </c>
+      <c r="P8" s="17">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q8" s="13" t="e">
+        <v>0.287438919229664</v>
+      </c>
+      <c r="Q8" s="17">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R8" s="13" t="e">
+        <v>2.38415406726071</v>
+      </c>
+      <c r="R8" s="17">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S8" s="14" t="e">
+        <v>0.0956493245185398</v>
+      </c>
+      <c r="S8" s="18">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.040118768259149</v>
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="7" t="s">
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="13" t="e">
+      <c r="D9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="13">
+        <v>6220800</v>
+      </c>
+      <c r="G9" s="14">
+        <v>8294472</v>
+      </c>
+      <c r="H9" s="11">
+        <v>82</v>
+      </c>
+      <c r="I9" s="15">
+        <v>186732</v>
+      </c>
+      <c r="J9" s="15">
+        <v>259464</v>
+      </c>
+      <c r="K9" s="11">
+        <v>0.269</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.004</v>
+      </c>
+      <c r="M9" s="11">
+        <v>3.212</v>
+      </c>
+      <c r="N9" s="11">
+        <v>0.004</v>
+      </c>
+      <c r="O9" s="16">
+        <v>3.489</v>
+      </c>
+      <c r="P9" s="17">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q9" s="13" t="e">
+        <v>0.286615075952995</v>
+      </c>
+      <c r="Q9" s="17">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R9" s="13" t="e">
+        <v>2.37732072226999</v>
+      </c>
+      <c r="R9" s="17">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S9" s="14" t="e">
+        <v>0.0743662940670679</v>
+      </c>
+      <c r="S9" s="18">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.0312815571624089</v>
       </c>
     </row>
     <row r="10" spans="1:19">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="13" t="e">
+      <c r="D10" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="13">
+        <v>6220800</v>
+      </c>
+      <c r="G10" s="14">
+        <v>8294472</v>
+      </c>
+      <c r="H10" s="11">
+        <v>52</v>
+      </c>
+      <c r="I10" s="15">
+        <v>127410</v>
+      </c>
+      <c r="J10" s="15">
+        <v>175964</v>
+      </c>
+      <c r="K10" s="11">
+        <v>0.265</v>
+      </c>
+      <c r="L10" s="11">
+        <v>0.004</v>
+      </c>
+      <c r="M10" s="11">
+        <v>3.183</v>
+      </c>
+      <c r="N10" s="11">
+        <v>0.003</v>
+      </c>
+      <c r="O10" s="16">
+        <v>3.455</v>
+      </c>
+      <c r="P10" s="17">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q10" s="13" t="e">
+        <v>0.289435600578871</v>
+      </c>
+      <c r="Q10" s="17">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R10" s="13" t="e">
+        <v>2.40071548480463</v>
+      </c>
+      <c r="R10" s="17">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S10" s="14" t="e">
+        <v>0.0509302460202605</v>
+      </c>
+      <c r="S10" s="18">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.0212146113700788</v>
       </c>
     </row>
     <row r="11" spans="1:19">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="13" t="e">
+      <c r="D11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="13">
+        <v>6220800</v>
+      </c>
+      <c r="G11" s="14">
+        <v>8294472</v>
+      </c>
+      <c r="H11" s="11">
+        <v>27</v>
+      </c>
+      <c r="I11" s="15">
+        <v>83460</v>
+      </c>
+      <c r="J11" s="15">
+        <v>114540</v>
+      </c>
+      <c r="K11" s="11">
+        <v>0.264</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0.004</v>
+      </c>
+      <c r="M11" s="11">
+        <v>3.171</v>
+      </c>
+      <c r="N11" s="11">
+        <v>0.002</v>
+      </c>
+      <c r="O11" s="16">
+        <v>3.441</v>
+      </c>
+      <c r="P11" s="17">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Q11" s="13" t="e">
+        <v>0.290613193839</v>
+      </c>
+      <c r="Q11" s="17">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="R11" s="13" t="e">
+        <v>2.41048299912816</v>
+      </c>
+      <c r="R11" s="17">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S11" s="14" t="e">
+        <v>0.0332868352223191</v>
+      </c>
+      <c r="S11" s="18">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.0138091972581257</v>
       </c>
     </row>
     <row r="12" spans="1:19">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="13" t="e">
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q12" s="13" t="e">
+      <c r="Q12" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R12" s="13" t="e">
+      <c r="R12" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S12" s="14" t="e">
+      <c r="S12" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:19">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="13" t="e">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q13" s="13" t="e">
+      <c r="Q13" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R13" s="13" t="e">
+      <c r="R13" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S13" s="14" t="e">
+      <c r="S13" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="7"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="13" t="e">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q14" s="13" t="e">
+      <c r="Q14" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R14" s="13" t="e">
+      <c r="R14" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S14" s="14" t="e">
+      <c r="S14" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="13" t="e">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q15" s="13" t="e">
+      <c r="Q15" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R15" s="13" t="e">
+      <c r="R15" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S15" s="14" t="e">
+      <c r="S15" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="13" t="e">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q16" s="13" t="e">
+      <c r="Q16" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R16" s="13" t="e">
+      <c r="R16" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S16" s="14" t="e">
+      <c r="S16" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="13" t="e">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="16"/>
+      <c r="P17" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q17" s="13" t="e">
+      <c r="Q17" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R17" s="13" t="e">
+      <c r="R17" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S17" s="14" t="e">
+      <c r="S17" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:19">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="13" t="e">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="16"/>
+      <c r="P18" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q18" s="13" t="e">
+      <c r="Q18" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R18" s="13" t="e">
+      <c r="R18" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S18" s="14" t="e">
+      <c r="S18" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:19">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
-      <c r="N19" s="7"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="13" t="e">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="16"/>
+      <c r="P19" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q19" s="13" t="e">
+      <c r="Q19" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R19" s="13" t="e">
+      <c r="R19" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S19" s="14" t="e">
+      <c r="S19" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="7"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="7"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="13" t="e">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="16"/>
+      <c r="P20" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q20" s="13" t="e">
+      <c r="Q20" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R20" s="13" t="e">
+      <c r="R20" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S20" s="14" t="e">
+      <c r="S20" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="7"/>
-      <c r="N21" s="7"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="13" t="e">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q21" s="13" t="e">
+      <c r="Q21" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R21" s="13" t="e">
+      <c r="R21" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S21" s="14" t="e">
+      <c r="S21" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
@@ -2214,428 +2394,818 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J13"/>
+      <selection activeCell="T2" sqref="T2:T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:10">
+    <row r="1" ht="18.75" spans="1:20">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" ht="144.75" spans="1:10">
+        <v>31</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" ht="144.75" spans="1:20">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" ht="72.75" spans="1:10">
+      <c r="K2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" ht="72.75" spans="1:20">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" ht="72.75" spans="1:10">
+      <c r="K3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" ht="72.75" spans="1:20">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B4" s="4">
         <v>11059200</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D4" s="4">
         <v>11059200</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F4" s="4">
         <v>11059200</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H4" s="4">
         <v>11059200</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J4" s="4">
         <v>11059200</v>
       </c>
-    </row>
-    <row r="5" ht="90.75" spans="1:10">
+      <c r="K4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" s="8">
+        <v>6220800</v>
+      </c>
+    </row>
+    <row r="5" ht="90.75" spans="1:20">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B5" s="4">
         <v>14745672</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D5" s="4">
         <v>14745672</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F5" s="4">
         <v>14745672</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="H5" s="4">
         <v>14745672</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J5" s="4">
         <v>14745672</v>
       </c>
-    </row>
-    <row r="6" ht="90.75" spans="1:10">
+      <c r="K5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="8">
+        <v>8294472</v>
+      </c>
+    </row>
+    <row r="6" ht="90.75" spans="1:20">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>169</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D6" s="3">
         <v>130</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="F6" s="3">
         <v>95</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H6" s="3">
         <v>58</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J6" s="3">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" ht="180.75" spans="1:10">
+      <c r="K6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" s="7">
+        <v>146</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="7">
+        <v>113</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P6" s="7">
+        <v>82</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="R6" s="7">
+        <v>52</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="T6" s="7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" ht="180.75" spans="1:20">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="F7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" ht="198.75" spans="1:10">
+        <v>42</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" ht="198.75" spans="1:20">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" ht="54.75" spans="1:10">
+        <v>53</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" ht="54.75" spans="1:20">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B9" s="3">
         <v>0.312</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D9" s="3">
         <v>0.309</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F9" s="3">
         <v>0.309</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="H9" s="3">
         <v>0.301</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="J9" s="3">
         <v>0.299</v>
       </c>
-    </row>
-    <row r="10" ht="72.75" spans="1:10">
+      <c r="K9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.274</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0.267</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0.269</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="R9" s="7">
+        <v>0.265</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="T9" s="7">
+        <v>0.264</v>
+      </c>
+    </row>
+    <row r="10" ht="72.75" spans="1:20">
       <c r="A10" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B10" s="3">
         <v>0.007</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="D10" s="3">
         <v>0.007</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="F10" s="3">
         <v>0.007</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="H10" s="3">
         <v>0.007</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="J10" s="3">
         <v>0.007</v>
       </c>
-    </row>
-    <row r="11" ht="54.75" spans="1:10">
+      <c r="K10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0.004</v>
+      </c>
+    </row>
+    <row r="11" ht="54.75" spans="1:20">
       <c r="A11" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B11" s="3">
         <v>3.293</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="D11" s="3">
         <v>3.286</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="F11" s="3">
         <v>3.272</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="H11" s="3">
         <v>3.218</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="J11" s="3">
         <v>3.178</v>
       </c>
-    </row>
-    <row r="12" ht="90.75" spans="1:10">
+      <c r="K11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" s="7">
+        <v>3.27</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="N11" s="7">
+        <v>3.202</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="7">
+        <v>3.212</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="R11" s="7">
+        <v>3.183</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="T11" s="7">
+        <v>3.171</v>
+      </c>
+    </row>
+    <row r="12" ht="90.75" spans="1:20">
       <c r="A12" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B12" s="3">
         <v>0.011</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="D12" s="3">
         <v>0.009</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="F12" s="3">
         <v>0.006</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="H12" s="3">
         <v>0.003</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="J12" s="3">
         <v>0.002</v>
       </c>
-    </row>
-    <row r="13" ht="54.75" spans="1:10">
+      <c r="K12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.007</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.006</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R12" s="7">
+        <v>0.003</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="T12" s="7">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="13" ht="54.75" spans="1:20">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B13" s="3">
         <v>3.623</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="D13" s="3">
         <v>3.611</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="F13" s="3">
         <v>3.594</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="H13" s="3">
         <v>3.529</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="J13" s="3">
         <v>3.486</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L13" s="7">
+        <v>3.555</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N13" s="7">
+        <v>3.479</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13" s="7">
+        <v>3.489</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="7">
+        <v>3.455</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" s="7">
+        <v>3.441</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
FInaliza testes da Cena 1 no Rpi 4 e inicia testes da Cena 1 no Rpi Zero
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -9,14 +9,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="RPI 4" sheetId="2" r:id="rId2"/>
+    <sheet name="RPI Z W" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="80">
   <si>
     <t>Scene</t>
   </si>
@@ -108,6 +109,39 @@
     <t>1080 x 1920</t>
   </si>
   <si>
+    <t>Min. Size Face: 1.6 / Scale Factor: 1.024 / Min. Neighbors: 4</t>
+  </si>
+  <si>
+    <t>720 x 1280</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Zero W</t>
+  </si>
+  <si>
+    <t>539,058 / 4.9%</t>
+  </si>
+  <si>
+    <t>742,472 / 5.0%</t>
+  </si>
+  <si>
+    <t>289,590 / 2.6%</t>
+  </si>
+  <si>
+    <t>399,528 / 2.7%</t>
+  </si>
+  <si>
+    <t>174,954 / 1.6%</t>
+  </si>
+  <si>
+    <t>241,748 / 1.6%</t>
+  </si>
+  <si>
+    <t>84,144 / 0.8%</t>
+  </si>
+  <si>
+    <t>115,868 / 0.8%</t>
+  </si>
+  <si>
     <t>Metric</t>
   </si>
   <si>
@@ -117,6 +151,9 @@
     <t>1.0 - Params</t>
   </si>
   <si>
+    <t>Min. Size Face: 1.5 / Scale Factor: 1.024 / Min. Neighbors: 3</t>
+  </si>
+  <si>
     <t>1.1 - Full Image Resolution</t>
   </si>
   <si>
@@ -132,21 +169,9 @@
     <t>1.5 - Cropped Faces Images Total Size (bytes) / (% from full image size)</t>
   </si>
   <si>
-    <t>539,058 / 4.9%</t>
-  </si>
-  <si>
     <t>408,060 / 3.7%</t>
   </si>
   <si>
-    <t>289,590 / 2.6%</t>
-  </si>
-  <si>
-    <t>174,954 / 1.6%</t>
-  </si>
-  <si>
-    <t>84,144 / 0.8%</t>
-  </si>
-  <si>
     <t>304,770 / 4.9%</t>
   </si>
   <si>
@@ -162,24 +187,30 @@
     <t>83,460 / 1.3%</t>
   </si>
   <si>
+    <t>83,553 / 3.0%</t>
+  </si>
+  <si>
+    <t>61,302 / 2.2%</t>
+  </si>
+  <si>
+    <t>44,025 / 1.6%</t>
+  </si>
+  <si>
+    <t>30,996 / 1.1%</t>
+  </si>
+  <si>
+    <t>22,491 / 0.8%</t>
+  </si>
+  <si>
+    <t>18,816 / 0.7%</t>
+  </si>
+  <si>
     <t>1.6 - Encoded Faces Images Total Size (bytes) / (% from full image encoded size)</t>
   </si>
   <si>
-    <t>742,472 / 5.0%</t>
-  </si>
-  <si>
     <t>562,352 / 3.8%</t>
   </si>
   <si>
-    <t>399,528 / 2.7%</t>
-  </si>
-  <si>
-    <t>241,748 / 1.6%</t>
-  </si>
-  <si>
-    <t>115,868 / 0.8%</t>
-  </si>
-  <si>
     <t>424,700 / 5.1%</t>
   </si>
   <si>
@@ -193,6 +224,24 @@
   </si>
   <si>
     <t>114,540 / 1.4%</t>
+  </si>
+  <si>
+    <t>117,928 / 3.2%</t>
+  </si>
+  <si>
+    <t>86,424 / 2.3%</t>
+  </si>
+  <si>
+    <t>61,884 / 1.7%</t>
+  </si>
+  <si>
+    <t>43,460 / 1.2%</t>
+  </si>
+  <si>
+    <t>31,228 / 0.8%</t>
+  </si>
+  <si>
+    <t>26,156 / 0.7%</t>
   </si>
   <si>
     <t>2.1 - Loading Image (s)</t>
@@ -216,12 +265,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.000"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="#,##0.000"/>
+    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -244,67 +293,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -333,6 +323,33 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -341,8 +358,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -363,13 +426,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -378,21 +434,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -427,7 +476,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -445,37 +554,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -487,79 +614,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -571,7 +644,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,31 +656,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -660,15 +709,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -684,6 +724,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -691,6 +746,15 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -725,21 +789,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -753,140 +802,140 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -930,7 +979,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -939,7 +988,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1335,17 +1384,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S21"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9037037037037" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.1111111111111" customWidth="1"/>
+    <col min="1" max="1" width="9.44444444444444" customWidth="1"/>
     <col min="2" max="2" width="10.1111111111111" customWidth="1"/>
-    <col min="3" max="3" width="13.1111111111111" customWidth="1"/>
+    <col min="3" max="3" width="17.2222222222222" customWidth="1"/>
     <col min="4" max="4" width="12.3333333333333" customWidth="1"/>
     <col min="5" max="7" width="13.1111111111111" customWidth="1"/>
     <col min="8" max="8" width="7.22222222222222" customWidth="1"/>
@@ -1528,19 +1577,19 @@
         <v>3.611</v>
       </c>
       <c r="P3" s="17">
-        <f t="shared" ref="P3:P21" si="0">1/O3</f>
+        <f t="shared" ref="P3:P36" si="0">1/O3</f>
         <v>0.27693159789532</v>
       </c>
       <c r="Q3" s="17">
-        <f t="shared" ref="Q3:Q21" si="1">G3*P3/1000000</f>
+        <f t="shared" ref="Q3:Q36" si="1">G3*P3/1000000</f>
         <v>4.08354250900028</v>
       </c>
       <c r="R3" s="17">
-        <f t="shared" ref="R3:R21" si="2">J3*P3/1000000</f>
+        <f t="shared" ref="R3:R36" si="2">J3*P3/1000000</f>
         <v>0.155733037939629</v>
       </c>
       <c r="S3" s="18">
-        <f t="shared" ref="S3:S21" si="3">R3/Q3</f>
+        <f t="shared" ref="S3:S36" si="3">R3/Q3</f>
         <v>0.0381367495492915</v>
       </c>
     </row>
@@ -2058,331 +2107,1120 @@
       <c r="C12" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="16"/>
-      <c r="P12" s="17" t="e">
+      <c r="D12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="13">
+        <v>2764800</v>
+      </c>
+      <c r="G12" s="14">
+        <v>3686472</v>
+      </c>
+      <c r="H12" s="11">
+        <v>52</v>
+      </c>
+      <c r="I12" s="15">
+        <v>83553</v>
+      </c>
+      <c r="J12" s="15">
+        <v>117928</v>
+      </c>
+      <c r="K12" s="11">
+        <v>0.116</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0.002</v>
+      </c>
+      <c r="M12" s="11">
+        <v>2.374</v>
+      </c>
+      <c r="N12" s="11">
+        <v>0.003</v>
+      </c>
+      <c r="O12" s="16">
+        <v>2.495</v>
+      </c>
+      <c r="P12" s="17">
+        <f t="shared" si="0"/>
+        <v>0.400801603206413</v>
+      </c>
+      <c r="Q12" s="17">
+        <f t="shared" si="1"/>
+        <v>1.47754388777555</v>
+      </c>
+      <c r="R12" s="17">
+        <f t="shared" si="2"/>
+        <v>0.0472657314629258</v>
+      </c>
+      <c r="S12" s="18">
+        <f t="shared" si="3"/>
+        <v>0.0319893925682875</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="13">
+        <v>2764800</v>
+      </c>
+      <c r="G13" s="14">
+        <v>3686472</v>
+      </c>
+      <c r="H13" s="11">
+        <v>37</v>
+      </c>
+      <c r="I13" s="15">
+        <v>61302</v>
+      </c>
+      <c r="J13" s="15">
+        <v>86424</v>
+      </c>
+      <c r="K13" s="11">
+        <v>0.126</v>
+      </c>
+      <c r="L13" s="11">
+        <v>0.002</v>
+      </c>
+      <c r="M13" s="11">
+        <v>2.362</v>
+      </c>
+      <c r="N13" s="11">
+        <v>0.003</v>
+      </c>
+      <c r="O13" s="16">
+        <v>2.493</v>
+      </c>
+      <c r="P13" s="17">
+        <f t="shared" si="0"/>
+        <v>0.401123144805455</v>
+      </c>
+      <c r="Q13" s="17">
+        <f t="shared" si="1"/>
+        <v>1.47872924187726</v>
+      </c>
+      <c r="R13" s="17">
+        <f t="shared" si="2"/>
+        <v>0.0346666666666667</v>
+      </c>
+      <c r="S13" s="18">
+        <f t="shared" si="3"/>
+        <v>0.0234435525347812</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="A14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="13">
+        <v>2764800</v>
+      </c>
+      <c r="G14" s="14">
+        <v>3686472</v>
+      </c>
+      <c r="H14" s="11">
+        <v>26</v>
+      </c>
+      <c r="I14" s="15">
+        <v>44025</v>
+      </c>
+      <c r="J14" s="15">
+        <v>61884</v>
+      </c>
+      <c r="K14" s="11">
+        <v>0.123</v>
+      </c>
+      <c r="L14" s="11">
+        <v>0.002</v>
+      </c>
+      <c r="M14" s="11">
+        <v>2.358</v>
+      </c>
+      <c r="N14" s="11">
+        <v>0.001</v>
+      </c>
+      <c r="O14" s="16">
+        <v>2.484</v>
+      </c>
+      <c r="P14" s="17">
+        <f t="shared" si="0"/>
+        <v>0.402576489533011</v>
+      </c>
+      <c r="Q14" s="17">
+        <f t="shared" si="1"/>
+        <v>1.48408695652174</v>
+      </c>
+      <c r="R14" s="17">
+        <f t="shared" si="2"/>
+        <v>0.0249130434782609</v>
+      </c>
+      <c r="S14" s="18">
+        <f t="shared" si="3"/>
+        <v>0.0167867815081737</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F15" s="13">
+        <v>2764800</v>
+      </c>
+      <c r="G15" s="14">
+        <v>3686472</v>
+      </c>
+      <c r="H15" s="11">
+        <v>17</v>
+      </c>
+      <c r="I15" s="15">
+        <v>30996</v>
+      </c>
+      <c r="J15" s="15">
+        <v>43460</v>
+      </c>
+      <c r="K15" s="11">
+        <v>0.118</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.002</v>
+      </c>
+      <c r="M15" s="11">
+        <v>2.362</v>
+      </c>
+      <c r="N15" s="11">
+        <v>0.001</v>
+      </c>
+      <c r="O15" s="16">
+        <v>2.483</v>
+      </c>
+      <c r="P15" s="17">
+        <f t="shared" si="0"/>
+        <v>0.402738622633911</v>
+      </c>
+      <c r="Q15" s="17">
+        <f t="shared" si="1"/>
+        <v>1.48468465565848</v>
+      </c>
+      <c r="R15" s="17">
+        <f t="shared" si="2"/>
+        <v>0.0175030205396698</v>
+      </c>
+      <c r="S15" s="18">
+        <f t="shared" si="3"/>
+        <v>0.0117890492590205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="A16" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="13">
+        <v>2764800</v>
+      </c>
+      <c r="G16" s="14">
+        <v>3686472</v>
+      </c>
+      <c r="H16" s="11">
+        <v>9</v>
+      </c>
+      <c r="I16" s="15">
+        <v>18816</v>
+      </c>
+      <c r="J16" s="15">
+        <v>26156</v>
+      </c>
+      <c r="K16" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0.002</v>
+      </c>
+      <c r="M16" s="11">
+        <v>2.348</v>
+      </c>
+      <c r="N16" s="11">
+        <v>0.001</v>
+      </c>
+      <c r="O16" s="16">
+        <v>2.476</v>
+      </c>
+      <c r="P16" s="17">
+        <f t="shared" si="0"/>
+        <v>0.403877221324717</v>
+      </c>
+      <c r="Q16" s="17">
+        <f t="shared" si="1"/>
+        <v>1.48888206785137</v>
+      </c>
+      <c r="R16" s="17">
+        <f t="shared" si="2"/>
+        <v>0.0105638126009693</v>
+      </c>
+      <c r="S16" s="18">
+        <f t="shared" si="3"/>
+        <v>0.00709513052045424</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="13">
+        <v>11059200</v>
+      </c>
+      <c r="G17" s="14">
+        <v>14745672</v>
+      </c>
+      <c r="H17" s="11">
+        <v>169</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="11">
+        <v>1.624</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0.13</v>
+      </c>
+      <c r="M17" s="11">
+        <v>93.5</v>
+      </c>
+      <c r="N17" s="11">
+        <v>0.092</v>
+      </c>
+      <c r="O17" s="16">
+        <v>95.346</v>
+      </c>
+      <c r="P17" s="17">
+        <f t="shared" si="0"/>
+        <v>0.0104881169634804</v>
+      </c>
+      <c r="Q17" s="17">
+        <f t="shared" si="1"/>
+        <v>0.154654332641118</v>
+      </c>
+      <c r="R17" s="17" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S17" s="18" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="13">
+        <v>11059200</v>
+      </c>
+      <c r="G18" s="14">
+        <v>14745672</v>
+      </c>
+      <c r="H18" s="11">
+        <v>130</v>
+      </c>
+      <c r="I18" s="15">
+        <v>408060</v>
+      </c>
+      <c r="J18" s="15">
+        <v>562352</v>
+      </c>
+      <c r="K18" s="11">
+        <v>1.631</v>
+      </c>
+      <c r="L18" s="11">
+        <v>0.208</v>
+      </c>
+      <c r="M18" s="11">
+        <v>92.359</v>
+      </c>
+      <c r="N18" s="11">
+        <v>0.081</v>
+      </c>
+      <c r="O18" s="16">
+        <v>94.279</v>
+      </c>
+      <c r="P18" s="17">
+        <f t="shared" si="0"/>
+        <v>0.010606815939923</v>
+      </c>
+      <c r="Q18" s="17">
+        <f t="shared" si="1"/>
+        <v>0.156404628814476</v>
+      </c>
+      <c r="R18" s="17">
+        <f t="shared" si="2"/>
+        <v>0.00596476415744758</v>
+      </c>
+      <c r="S18" s="18">
+        <f t="shared" si="3"/>
+        <v>0.0381367495492915</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="13">
+        <v>11059200</v>
+      </c>
+      <c r="G19" s="14">
+        <v>14745672</v>
+      </c>
+      <c r="H19" s="11">
+        <v>95</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="J19" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="K19" s="11">
+        <v>1.619</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0.125</v>
+      </c>
+      <c r="M19" s="11">
+        <v>91.214</v>
+      </c>
+      <c r="N19" s="11">
+        <v>0.049</v>
+      </c>
+      <c r="O19" s="16">
+        <v>93.007</v>
+      </c>
+      <c r="P19" s="17">
+        <f t="shared" si="0"/>
+        <v>0.0107518788908362</v>
+      </c>
+      <c r="Q19" s="17">
+        <f t="shared" si="1"/>
+        <v>0.158543679507994</v>
+      </c>
+      <c r="R19" s="17" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S19" s="18" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="13">
+        <v>11059200</v>
+      </c>
+      <c r="G20" s="14">
+        <v>14745672</v>
+      </c>
+      <c r="H20" s="11">
+        <v>58</v>
+      </c>
+      <c r="I20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="11">
+        <v>1.644</v>
+      </c>
+      <c r="L20" s="11">
+        <v>0.127</v>
+      </c>
+      <c r="M20" s="11">
+        <v>90.538</v>
+      </c>
+      <c r="N20" s="11">
+        <v>0.041</v>
+      </c>
+      <c r="O20" s="16">
+        <v>92.35</v>
+      </c>
+      <c r="P20" s="17">
+        <f t="shared" si="0"/>
+        <v>0.0108283703302653</v>
+      </c>
+      <c r="Q20" s="17">
+        <f t="shared" si="1"/>
+        <v>0.159671597184624</v>
+      </c>
+      <c r="R20" s="17" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S20" s="18" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="13">
+        <v>11059200</v>
+      </c>
+      <c r="G21" s="14">
+        <v>14745672</v>
+      </c>
+      <c r="H21" s="11">
+        <v>25</v>
+      </c>
+      <c r="I21" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="K21" s="11">
+        <v>1.611</v>
+      </c>
+      <c r="L21" s="11">
+        <v>0.156</v>
+      </c>
+      <c r="M21" s="11">
+        <v>89.549</v>
+      </c>
+      <c r="N21" s="11">
+        <v>0.014</v>
+      </c>
+      <c r="O21" s="16">
+        <v>91.33</v>
+      </c>
+      <c r="P21" s="17">
+        <f t="shared" si="0"/>
+        <v>0.0109493047191503</v>
+      </c>
+      <c r="Q21" s="17">
+        <f t="shared" si="1"/>
+        <v>0.161454856016643</v>
+      </c>
+      <c r="R21" s="17" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S21" s="18" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="16"/>
+      <c r="P22" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q12" s="17" t="e">
+      <c r="Q22" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R12" s="17" t="e">
+      <c r="R22" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S12" s="18" t="e">
+      <c r="S22" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="17" t="e">
+    <row r="23" spans="1:19">
+      <c r="A23" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="16"/>
+      <c r="P23" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q13" s="17" t="e">
+      <c r="Q23" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R13" s="17" t="e">
+      <c r="R23" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S13" s="18" t="e">
+      <c r="S23" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
-      <c r="A14" s="12"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="17" t="e">
+    <row r="24" spans="1:19">
+      <c r="A24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="16"/>
+      <c r="P24" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q14" s="17" t="e">
+      <c r="Q24" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R14" s="17" t="e">
+      <c r="R24" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S14" s="18" t="e">
+      <c r="S24" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="12"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="16"/>
-      <c r="P15" s="17" t="e">
+    <row r="25" spans="1:19">
+      <c r="A25" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="16"/>
+      <c r="P25" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q15" s="17" t="e">
+      <c r="Q25" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R15" s="17" t="e">
+      <c r="R25" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S15" s="18" t="e">
+      <c r="S25" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="16"/>
-      <c r="P16" s="17" t="e">
+    <row r="26" spans="1:19">
+      <c r="A26" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="16"/>
+      <c r="P26" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q16" s="17" t="e">
+      <c r="Q26" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R16" s="17" t="e">
+      <c r="R26" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S16" s="18" t="e">
+      <c r="S26" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="12"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="15"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="17" t="e">
+    <row r="27" spans="1:19">
+      <c r="A27" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q17" s="17" t="e">
+      <c r="Q27" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R17" s="17" t="e">
+      <c r="R27" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S17" s="18" t="e">
+      <c r="S27" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="16"/>
-      <c r="P18" s="17" t="e">
+    <row r="28" spans="1:19">
+      <c r="A28" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="16"/>
+      <c r="P28" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q18" s="17" t="e">
+      <c r="Q28" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R18" s="17" t="e">
+      <c r="R28" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S18" s="18" t="e">
+      <c r="S28" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="12"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="16"/>
-      <c r="P19" s="17" t="e">
+    <row r="29" spans="1:19">
+      <c r="A29" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="16"/>
+      <c r="P29" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q19" s="17" t="e">
+      <c r="Q29" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R19" s="17" t="e">
+      <c r="R29" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S19" s="18" t="e">
+      <c r="S29" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="12"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="16"/>
-      <c r="P20" s="17" t="e">
+    <row r="30" spans="1:19">
+      <c r="A30" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="16"/>
+      <c r="P30" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q20" s="17" t="e">
+      <c r="Q30" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R20" s="17" t="e">
+      <c r="R30" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S20" s="18" t="e">
+      <c r="S30" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="12"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="16"/>
-      <c r="P21" s="17" t="e">
+    <row r="31" spans="1:19">
+      <c r="A31" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="16"/>
+      <c r="P31" s="17" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q21" s="17" t="e">
+      <c r="Q31" s="17" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="R21" s="17" t="e">
+      <c r="R31" s="17" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="S21" s="18" t="e">
+      <c r="S31" s="18" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
+    </row>
+    <row r="32" spans="1:19">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="16"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="17"/>
+      <c r="R32" s="17"/>
+      <c r="S32" s="18"/>
+    </row>
+    <row r="33" spans="1:19">
+      <c r="A33" s="11"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="18"/>
+    </row>
+    <row r="34" spans="1:19">
+      <c r="A34" s="11"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="17"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="18"/>
+    </row>
+    <row r="35" spans="1:19">
+      <c r="A35" s="11"/>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="18"/>
+    </row>
+    <row r="36" spans="1:19">
+      <c r="A36" s="11"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="17"/>
+      <c r="Q36" s="17"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2394,818 +3232,1722 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:T13"/>
+  <dimension ref="A1:AF13"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2:T13"/>
+    <sheetView topLeftCell="M8" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2:AF13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:20">
+    <row r="1" ht="18.75" spans="1:32">
+      <c r="A1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" ht="144.75" spans="1:32">
+      <c r="A2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" ht="72.75" spans="1:32">
+      <c r="A3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" ht="72.75" spans="1:32">
+      <c r="A4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="8">
+        <v>11059200</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="8">
+        <v>11059200</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="8">
+        <v>11059200</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="8">
+        <v>11059200</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="8">
+        <v>11059200</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="T4" s="8">
+        <v>6220800</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V4" s="4">
+        <v>2764800</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="X4" s="4">
+        <v>2764800</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z4" s="4">
+        <v>2764800</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>2764800</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD4" s="4">
+        <v>2764800</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF4" s="4">
+        <v>2764800</v>
+      </c>
+    </row>
+    <row r="5" ht="90.75" spans="1:32">
+      <c r="A5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="8">
+        <v>14745672</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="8">
+        <v>14745672</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="8">
+        <v>14745672</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="8">
+        <v>14745672</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="8">
+        <v>14745672</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="P5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="R5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="T5" s="8">
+        <v>8294472</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V5" s="4">
+        <v>3686472</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="X5" s="4">
+        <v>3686472</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z5" s="4">
+        <v>3686472</v>
+      </c>
+      <c r="AA5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>3686472</v>
+      </c>
+      <c r="AC5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD5" s="4">
+        <v>3686472</v>
+      </c>
+      <c r="AE5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>3686472</v>
+      </c>
+    </row>
+    <row r="6" ht="90.75" spans="1:32">
+      <c r="A6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="7">
+        <v>169</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="7">
+        <v>130</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="7">
+        <v>95</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="7">
+        <v>58</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="7">
+        <v>25</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L6" s="7">
+        <v>146</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="7">
+        <v>113</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6" s="7">
+        <v>82</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" s="7">
+        <v>52</v>
+      </c>
+      <c r="S6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="T6" s="7">
+        <v>27</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V6" s="3">
+        <v>52</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="X6" s="3">
+        <v>37</v>
+      </c>
+      <c r="Y6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>26</v>
+      </c>
+      <c r="AA6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>17</v>
+      </c>
+      <c r="AC6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>11</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF6" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" ht="180.75" spans="1:32">
+      <c r="A7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="R7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="V7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AD7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" ht="198.75" spans="1:32">
+      <c r="A8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="R8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="T8" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="V8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="X8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="AC8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" ht="54.75" spans="1:32">
+      <c r="A9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0.312</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.309</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="7">
+        <v>0.309</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="7">
+        <v>0.301</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.299</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.274</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0.267</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0.269</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="R9" s="7">
+        <v>0.265</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="T9" s="7">
+        <v>0.264</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="V9" s="3">
+        <v>0.116</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0.126</v>
+      </c>
+      <c r="Y9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0.123</v>
+      </c>
+      <c r="AA9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>0.118</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>0.12</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF9" s="3">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="10" ht="72.75" spans="1:32">
+      <c r="A10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.007</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.007</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.007</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0.007</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0.007</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="R10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="S10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="T10" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="V10" s="3">
+        <v>0.002</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0.002</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0.002</v>
+      </c>
+      <c r="AA10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>0.002</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>0.002</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF10" s="3">
+        <v>0.002</v>
+      </c>
+    </row>
+    <row r="11" ht="54.75" spans="1:32">
+      <c r="A11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="7">
+        <v>3.293</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="7">
+        <v>3.286</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F11" s="7">
+        <v>3.272</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="7">
+        <v>3.218</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="7">
+        <v>3.178</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" s="7">
+        <v>3.27</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N11" s="7">
+        <v>3.202</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P11" s="7">
+        <v>3.212</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="R11" s="7">
+        <v>3.183</v>
+      </c>
+      <c r="S11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="T11" s="7">
+        <v>3.171</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="V11" s="3">
+        <v>2.374</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="X11" s="3">
+        <v>2.362</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>2.358</v>
+      </c>
+      <c r="AA11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>2.362</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>2.351</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AF11" s="3">
+        <v>2.348</v>
+      </c>
+    </row>
+    <row r="12" ht="90.75" spans="1:32">
+      <c r="A12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.011</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.009</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.006</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.003</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.002</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.007</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.006</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0.004</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="R12" s="7">
+        <v>0.003</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="T12" s="7">
+        <v>0.002</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="V12" s="3">
+        <v>0.003</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="X12" s="3">
+        <v>0.003</v>
+      </c>
+      <c r="Y12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="AA12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>0.001</v>
+      </c>
+      <c r="AE12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF12" s="3">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="13" ht="54.75" spans="1:32">
+      <c r="A13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="7">
+        <v>3.623</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="7">
+        <v>3.611</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="7">
+        <v>3.594</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="7">
+        <v>3.529</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="7">
+        <v>3.486</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="L13" s="7">
+        <v>3.555</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="N13" s="7">
+        <v>3.479</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="P13" s="7">
+        <v>3.489</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="R13" s="7">
+        <v>3.455</v>
+      </c>
+      <c r="S13" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="T13" s="7">
+        <v>3.441</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="V13" s="3">
+        <v>2.495</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X13" s="3">
+        <v>2.493</v>
+      </c>
+      <c r="Y13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>2.484</v>
+      </c>
+      <c r="AA13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>2.483</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>2.474</v>
+      </c>
+      <c r="AE13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF13" s="3">
+        <v>2.476</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.4444444444444" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="16384" width="11.4444444444444" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18.75" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" ht="144.75" spans="1:20">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" ht="90.75" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" ht="72.75" spans="1:20">
+    </row>
+    <row r="3" ht="54.75" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T3" s="7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" ht="72.75" spans="1:20">
+    </row>
+    <row r="4" ht="54.75" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="B4" s="4">
         <v>11059200</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="4">
-        <v>11059200</v>
+        <v>46</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F4" s="4">
         <v>11059200</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="H4" s="4">
         <v>11059200</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="J4" s="4">
         <v>11059200</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="8">
-        <v>6220800</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="8">
-        <v>6220800</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="8">
-        <v>6220800</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="R4" s="8">
-        <v>6220800</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="T4" s="8">
-        <v>6220800</v>
-      </c>
-    </row>
-    <row r="5" ht="90.75" spans="1:20">
+    </row>
+    <row r="5" ht="72.75" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B5" s="4">
         <v>14745672</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="4">
-        <v>14745672</v>
+        <v>47</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="F5" s="4">
         <v>14745672</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="H5" s="4">
         <v>14745672</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="J5" s="4">
         <v>14745672</v>
       </c>
-      <c r="K5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="8">
-        <v>8294472</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N5" s="8">
-        <v>8294472</v>
-      </c>
-      <c r="O5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="P5" s="8">
-        <v>8294472</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="R5" s="8">
-        <v>8294472</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T5" s="8">
-        <v>8294472</v>
-      </c>
-    </row>
-    <row r="6" ht="90.75" spans="1:20">
+    </row>
+    <row r="6" ht="54.75" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B6" s="3">
         <v>169</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="3">
-        <v>130</v>
+        <v>48</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="F6" s="3">
         <v>95</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="H6" s="3">
         <v>58</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="J6" s="3">
         <v>25</v>
       </c>
-      <c r="K6" s="6" t="s">
+    </row>
+    <row r="7" ht="144.75" spans="1:10">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" ht="162.75" spans="1:10">
+      <c r="A8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="7">
-        <v>146</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="7">
-        <v>113</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="7">
-        <v>82</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="7">
-        <v>52</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="T6" s="7">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" ht="180.75" spans="1:20">
-      <c r="A7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="G8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="I8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L7" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" ht="198.75" spans="1:20">
-      <c r="A8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N8" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="T8" s="7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" ht="54.75" spans="1:20">
+    </row>
+    <row r="9" ht="36.75" spans="1:10">
       <c r="A9" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B9" s="3">
-        <v>0.312</v>
+        <v>1.624</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.309</v>
+        <v>75</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F9" s="3">
-        <v>0.309</v>
+        <v>1.619</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="H9" s="3">
-        <v>0.301</v>
+        <v>1.644</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="J9" s="3">
-        <v>0.299</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="L9" s="7">
-        <v>0.274</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N9" s="7">
-        <v>0.267</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="P9" s="7">
-        <v>0.269</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="R9" s="7">
-        <v>0.265</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="T9" s="7">
-        <v>0.264</v>
-      </c>
-    </row>
-    <row r="10" ht="72.75" spans="1:20">
+        <v>1.611</v>
+      </c>
+    </row>
+    <row r="10" ht="54.75" spans="1:10">
       <c r="A10" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B10" s="3">
-        <v>0.007</v>
+        <v>0.13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" s="3">
-        <v>0.007</v>
+        <v>76</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="F10" s="3">
-        <v>0.007</v>
+        <v>0.125</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="H10" s="3">
-        <v>0.007</v>
+        <v>0.127</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="J10" s="3">
-        <v>0.007</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="L10" s="7">
-        <v>0.004</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N10" s="7">
-        <v>0.004</v>
-      </c>
-      <c r="O10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="P10" s="7">
-        <v>0.004</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="R10" s="7">
-        <v>0.004</v>
-      </c>
-      <c r="S10" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="T10" s="7">
-        <v>0.004</v>
-      </c>
-    </row>
-    <row r="11" ht="54.75" spans="1:20">
+        <v>0.156</v>
+      </c>
+    </row>
+    <row r="11" ht="36.75" spans="1:10">
       <c r="A11" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="B11" s="3">
-        <v>3.293</v>
+        <v>93.5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="3">
-        <v>3.286</v>
+        <v>77</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="F11" s="3">
-        <v>3.272</v>
+        <v>91.214</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="H11" s="3">
-        <v>3.218</v>
+        <v>90.538</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="J11" s="3">
-        <v>3.178</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" s="7">
-        <v>3.27</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="N11" s="7">
-        <v>3.202</v>
-      </c>
-      <c r="O11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P11" s="7">
-        <v>3.212</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="R11" s="7">
-        <v>3.183</v>
-      </c>
-      <c r="S11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="T11" s="7">
-        <v>3.171</v>
-      </c>
-    </row>
-    <row r="12" ht="90.75" spans="1:20">
+        <v>89.549</v>
+      </c>
+    </row>
+    <row r="12" ht="72.75" spans="1:10">
       <c r="A12" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="B12" s="3">
-        <v>0.011</v>
+        <v>0.092</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.009</v>
+        <v>78</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="F12" s="3">
-        <v>0.006</v>
+        <v>0.049</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="H12" s="3">
-        <v>0.003</v>
+        <v>0.041</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="J12" s="3">
-        <v>0.002</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="L12" s="7">
-        <v>0.007</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N12" s="7">
-        <v>0.006</v>
-      </c>
-      <c r="O12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="P12" s="7">
-        <v>0.004</v>
-      </c>
-      <c r="Q12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="R12" s="7">
-        <v>0.003</v>
-      </c>
-      <c r="S12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="T12" s="7">
-        <v>0.002</v>
-      </c>
-    </row>
-    <row r="13" ht="54.75" spans="1:20">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="13" ht="54.75" spans="1:10">
       <c r="A13" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B13" s="3">
-        <v>3.623</v>
+        <v>95.346</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="3">
-        <v>3.611</v>
+        <v>79</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="F13" s="3">
-        <v>3.594</v>
+        <v>93.007</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="H13" s="3">
-        <v>3.529</v>
+        <v>92.35</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="J13" s="3">
-        <v>3.486</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="L13" s="7">
-        <v>3.555</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="N13" s="7">
-        <v>3.479</v>
-      </c>
-      <c r="O13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="P13" s="7">
-        <v>3.489</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="R13" s="7">
-        <v>3.455</v>
-      </c>
-      <c r="S13" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="T13" s="7">
-        <v>3.441</v>
+        <v>91.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continuando experimentos Cena 2 e testando no Raspberry Piu Zero
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12555" tabRatio="500" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="12555" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cena 1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="110">
   <si>
     <t>Scene</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>240x320</t>
+  </si>
+  <si>
+    <t>RpiZ</t>
   </si>
 </sst>
 </file>
@@ -353,14 +356,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="0.000_ "/>
-    <numFmt numFmtId="178" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0.000"/>
+    <numFmt numFmtId="177" formatCode="#,##0.00_ "/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="0.000_ "/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="#,##0.000"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -383,24 +386,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -415,17 +402,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -434,11 +413,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -449,15 +427,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -468,6 +448,43 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -486,16 +503,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -506,36 +539,6 @@
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -572,13 +575,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -590,19 +587,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,49 +665,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,7 +677,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -686,7 +695,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,31 +743,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,25 +755,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,11 +799,28 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,15 +830,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -838,43 +849,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -893,145 +872,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="28" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyBorder="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1078,7 +1081,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1087,19 +1090,19 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="2" xfId="47" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1108,7 +1111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1117,7 +1120,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4081,8 +4084,8 @@
   <sheetPr/>
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.9037037037037" defaultRowHeight="15"/>
@@ -4219,23 +4222,23 @@
         <v>0.082</v>
       </c>
       <c r="Q2" s="20">
-        <f>SUM(M2:O2,K2)</f>
+        <f t="shared" ref="Q2:Q7" si="0">SUM(M2:O2,K2)</f>
         <v>0.114</v>
       </c>
       <c r="R2" s="21">
-        <f>1/Q2</f>
+        <f t="shared" ref="R2:R7" si="1">1/Q2</f>
         <v>8.7719298245614</v>
       </c>
       <c r="S2" s="21">
-        <f>G2*R2/1000000</f>
+        <f t="shared" ref="S2:S7" si="2">G2*R2/1000000</f>
         <v>16.8427368421053</v>
       </c>
       <c r="T2" s="21">
-        <f>J2*R2/1000000</f>
+        <f t="shared" ref="T2:T7" si="3">J2*R2/1000000</f>
         <v>1.57017543859649</v>
       </c>
       <c r="U2" s="22">
-        <f>T2/S2</f>
+        <f t="shared" ref="U2:U7" si="4">T2/S2</f>
         <v>0.0932256707040153</v>
       </c>
     </row>
@@ -4289,23 +4292,23 @@
         <v>0.06</v>
       </c>
       <c r="Q3" s="20">
-        <f>SUM(M3:O3,K3)</f>
+        <f t="shared" si="0"/>
         <v>0.098</v>
       </c>
       <c r="R3" s="21">
-        <f>1/Q3</f>
+        <f t="shared" si="1"/>
         <v>10.2040816326531</v>
       </c>
       <c r="S3" s="21">
-        <f>G3*R3/1000000</f>
+        <f t="shared" si="2"/>
         <v>12.5395102040816</v>
       </c>
       <c r="T3" s="21">
-        <f>J3*R3/1000000</f>
+        <f t="shared" si="3"/>
         <v>0.943755102040816</v>
       </c>
       <c r="U3" s="22">
-        <f>T3/S3</f>
+        <f t="shared" si="4"/>
         <v>0.0752625171702179</v>
       </c>
     </row>
@@ -4359,23 +4362,23 @@
         <v>0.025</v>
       </c>
       <c r="Q4" s="20">
-        <f>SUM(M4:O4,K4)</f>
+        <f t="shared" si="0"/>
         <v>0.079</v>
       </c>
       <c r="R4" s="21">
-        <f>1/Q4</f>
+        <f t="shared" si="1"/>
         <v>12.6582278481013</v>
       </c>
       <c r="S4" s="21">
-        <f>G4*R4/1000000</f>
+        <f t="shared" si="2"/>
         <v>3.88951898734177</v>
       </c>
       <c r="T4" s="21">
-        <f>J4*R4/1000000</f>
+        <f t="shared" si="3"/>
         <v>0.36820253164557</v>
       </c>
       <c r="U4" s="22">
-        <f>T4/S4</f>
+        <f t="shared" si="4"/>
         <v>0.0946653128173084</v>
       </c>
     </row>
@@ -4389,38 +4392,64 @@
       <c r="C5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="16"/>
-      <c r="J5" s="16"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="19"/>
+      <c r="D5" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="14">
+        <v>1440000</v>
+      </c>
+      <c r="G5" s="15">
+        <v>1920072</v>
+      </c>
+      <c r="H5" s="12">
+        <v>1</v>
+      </c>
+      <c r="I5" s="16">
+        <v>133563</v>
+      </c>
+      <c r="J5" s="16">
+        <v>179000</v>
+      </c>
+      <c r="K5" s="18">
+        <v>0.099</v>
+      </c>
+      <c r="L5" s="18">
+        <v>0.265</v>
+      </c>
+      <c r="M5" s="12">
+        <v>0.015</v>
+      </c>
+      <c r="N5" s="12">
+        <v>0.453</v>
+      </c>
+      <c r="O5" s="12">
+        <v>0.006</v>
+      </c>
+      <c r="P5" s="12">
+        <v>0.739</v>
+      </c>
       <c r="Q5" s="20">
-        <f>SUM(M5:O5,K5)</f>
-        <v>0</v>
-      </c>
-      <c r="R5" s="21" t="e">
-        <f>1/Q5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S5" s="21" t="e">
-        <f>G5*R5/1000000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T5" s="21" t="e">
-        <f>J5*R5/1000000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U5" s="22" t="e">
-        <f>T5/S5</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v>0.573</v>
+      </c>
+      <c r="R5" s="21">
+        <f t="shared" si="1"/>
+        <v>1.74520069808028</v>
+      </c>
+      <c r="S5" s="21">
+        <f t="shared" si="2"/>
+        <v>3.3509109947644</v>
+      </c>
+      <c r="T5" s="21">
+        <f t="shared" si="3"/>
+        <v>0.31239092495637</v>
+      </c>
+      <c r="U5" s="22">
+        <f t="shared" si="4"/>
+        <v>0.0932256707040153</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -4433,38 +4462,64 @@
       <c r="C6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="19"/>
+      <c r="D6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="14">
+        <v>921600</v>
+      </c>
+      <c r="G6" s="15">
+        <v>1228872</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="16">
+        <v>69312</v>
+      </c>
+      <c r="J6" s="16">
+        <v>92488</v>
+      </c>
+      <c r="K6" s="18">
+        <v>0.094</v>
+      </c>
+      <c r="L6" s="18">
+        <v>0.161</v>
+      </c>
+      <c r="M6" s="18">
+        <v>0.012</v>
+      </c>
+      <c r="N6" s="12">
+        <v>0.257</v>
+      </c>
+      <c r="O6" s="12">
+        <v>0.004</v>
+      </c>
+      <c r="P6" s="12">
+        <v>0.434</v>
+      </c>
       <c r="Q6" s="20">
-        <f>SUM(M6:O6,K6)</f>
-        <v>0</v>
-      </c>
-      <c r="R6" s="21" t="e">
-        <f>1/Q6</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S6" s="21" t="e">
-        <f>G6*R6/1000000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T6" s="21" t="e">
-        <f>J6*R6/1000000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U6" s="22" t="e">
-        <f>T6/S6</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v>0.367</v>
+      </c>
+      <c r="R6" s="21">
+        <f t="shared" si="1"/>
+        <v>2.72479564032698</v>
+      </c>
+      <c r="S6" s="21">
+        <f t="shared" si="2"/>
+        <v>3.34842506811989</v>
+      </c>
+      <c r="T6" s="21">
+        <f t="shared" si="3"/>
+        <v>0.252010899182561</v>
+      </c>
+      <c r="U6" s="22">
+        <f t="shared" si="4"/>
+        <v>0.0752625171702179</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -4477,38 +4532,64 @@
       <c r="C7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="19"/>
+      <c r="D7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="14">
+        <v>230400</v>
+      </c>
+      <c r="G7" s="15">
+        <v>307272</v>
+      </c>
+      <c r="H7" s="12">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16">
+        <v>21675</v>
+      </c>
+      <c r="J7" s="16">
+        <v>29088</v>
+      </c>
+      <c r="K7" s="18">
+        <v>0.072</v>
+      </c>
+      <c r="L7" s="18">
+        <v>0.059</v>
+      </c>
+      <c r="M7" s="12">
+        <v>0.003</v>
+      </c>
+      <c r="N7" s="12">
+        <v>0.298</v>
+      </c>
+      <c r="O7" s="12">
+        <v>0.001</v>
+      </c>
+      <c r="P7" s="12">
+        <v>0.361</v>
+      </c>
       <c r="Q7" s="20">
-        <f>SUM(M7:O7,K7)</f>
-        <v>0</v>
-      </c>
-      <c r="R7" s="21" t="e">
-        <f>1/Q7</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="S7" s="21" t="e">
-        <f>G7*R7/1000000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T7" s="21" t="e">
-        <f>J7*R7/1000000</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="U7" s="22" t="e">
-        <f>T7/S7</f>
-        <v>#DIV/0!</v>
+        <f t="shared" si="0"/>
+        <v>0.374</v>
+      </c>
+      <c r="R7" s="21">
+        <f t="shared" si="1"/>
+        <v>2.67379679144385</v>
+      </c>
+      <c r="S7" s="21">
+        <f t="shared" si="2"/>
+        <v>0.821582887700535</v>
+      </c>
+      <c r="T7" s="21">
+        <f t="shared" si="3"/>
+        <v>0.0777754010695187</v>
+      </c>
+      <c r="U7" s="22">
+        <f t="shared" si="4"/>
+        <v>0.0946653128173084</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -4741,22 +4822,22 @@
       <c r="AF1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AK1" s="6" t="s">
+      <c r="AK1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AL1" s="6" t="s">
+      <c r="AL1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AM1" s="6" t="s">
+      <c r="AM1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="AN1" s="6" t="s">
+      <c r="AN1" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -4857,22 +4938,22 @@
       <c r="AF2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="7" t="s">
+      <c r="AI2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AK2" s="7" t="s">
+      <c r="AK2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AL2" s="8" t="s">
+      <c r="AL2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AM2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AN2" s="8" t="s">
+      <c r="AN2" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -4973,22 +5054,22 @@
       <c r="AF3" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI3" s="7" t="s">
+      <c r="AI3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AJ3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AK3" s="7" t="s">
+      <c r="AK3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AL3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AM3" s="7" t="s">
+      <c r="AM3" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AN3" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -5089,22 +5170,22 @@
       <c r="AF4" s="5">
         <v>2764800</v>
       </c>
-      <c r="AI4" s="7" t="s">
+      <c r="AI4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AJ4" s="9">
+      <c r="AJ4" s="5">
         <v>1440000</v>
       </c>
-      <c r="AK4" s="7" t="s">
+      <c r="AK4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AL4" s="9">
+      <c r="AL4" s="5">
         <v>921600</v>
       </c>
-      <c r="AM4" s="7" t="s">
+      <c r="AM4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AN4" s="9">
+      <c r="AN4" s="5">
         <v>230400</v>
       </c>
     </row>
@@ -5205,22 +5286,22 @@
       <c r="AF5" s="5">
         <v>3686472</v>
       </c>
-      <c r="AI5" s="7" t="s">
+      <c r="AI5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AJ5" s="9">
+      <c r="AJ5" s="5">
         <v>1920072</v>
       </c>
-      <c r="AK5" s="7" t="s">
+      <c r="AK5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AL5" s="9">
+      <c r="AL5" s="5">
         <v>1228872</v>
       </c>
-      <c r="AM5" s="7" t="s">
+      <c r="AM5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AN5" s="9">
+      <c r="AN5" s="5">
         <v>307272</v>
       </c>
     </row>
@@ -5321,22 +5402,22 @@
       <c r="AF6" s="4">
         <v>9</v>
       </c>
-      <c r="AI6" s="7" t="s">
+      <c r="AI6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AJ6" s="8">
+      <c r="AJ6" s="4">
         <v>1</v>
       </c>
-      <c r="AK6" s="7" t="s">
+      <c r="AK6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AL6" s="8">
+      <c r="AL6" s="4">
         <v>1</v>
       </c>
-      <c r="AM6" s="7" t="s">
+      <c r="AM6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AN6" s="8">
+      <c r="AN6" s="4">
         <v>1</v>
       </c>
     </row>
@@ -5437,22 +5518,22 @@
       <c r="AF7" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AI7" s="7" t="s">
+      <c r="AI7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AJ7" s="8" t="s">
+      <c r="AJ7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AK7" s="7" t="s">
+      <c r="AK7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AL7" s="8" t="s">
+      <c r="AL7" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AM7" s="7" t="s">
+      <c r="AM7" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="AN7" s="8" t="s">
+      <c r="AN7" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -5553,22 +5634,22 @@
       <c r="AF8" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="AI8" s="7" t="s">
+      <c r="AI8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AJ8" s="8" t="s">
+      <c r="AJ8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="AK8" s="7" t="s">
+      <c r="AK8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AL8" s="8" t="s">
+      <c r="AL8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AM8" s="7" t="s">
+      <c r="AM8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="AN8" s="8" t="s">
+      <c r="AN8" s="4" t="s">
         <v>89</v>
       </c>
     </row>
@@ -5669,22 +5750,22 @@
       <c r="AF9" s="4">
         <v>0.125</v>
       </c>
-      <c r="AI9" s="7" t="s">
+      <c r="AI9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AJ9" s="8">
+      <c r="AJ9" s="4">
         <v>0.062</v>
       </c>
-      <c r="AK9" s="7" t="s">
+      <c r="AK9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AL9" s="8">
+      <c r="AL9" s="4">
         <v>0.045</v>
       </c>
-      <c r="AM9" s="7" t="s">
+      <c r="AM9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="AN9" s="8">
+      <c r="AN9" s="4">
         <v>0.008</v>
       </c>
     </row>
@@ -5785,22 +5866,22 @@
       <c r="AF10" s="4">
         <v>0.002</v>
       </c>
-      <c r="AI10" s="7" t="s">
+      <c r="AI10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AJ10" s="8">
+      <c r="AJ10" s="4">
         <v>0.001</v>
       </c>
-      <c r="AK10" s="7" t="s">
+      <c r="AK10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AL10" s="8">
+      <c r="AL10" s="4">
         <v>0.001</v>
       </c>
-      <c r="AM10" s="7" t="s">
+      <c r="AM10" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="AN10" s="8">
+      <c r="AN10" s="4">
         <v>0</v>
       </c>
     </row>
@@ -5901,22 +5982,22 @@
       <c r="AF11" s="4">
         <v>2.348</v>
       </c>
-      <c r="AI11" s="7" t="s">
+      <c r="AI11" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AJ11" s="8">
+      <c r="AJ11" s="4">
         <v>0.017</v>
       </c>
-      <c r="AK11" s="7" t="s">
+      <c r="AK11" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AL11" s="8">
+      <c r="AL11" s="4">
         <v>0.013</v>
       </c>
-      <c r="AM11" s="7" t="s">
+      <c r="AM11" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AN11" s="8">
+      <c r="AN11" s="4">
         <v>0.017</v>
       </c>
     </row>
@@ -6017,22 +6098,22 @@
       <c r="AF12" s="4">
         <v>0.001</v>
       </c>
-      <c r="AI12" s="7" t="s">
+      <c r="AI12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AJ12" s="8">
+      <c r="AJ12" s="4">
         <v>0.002</v>
       </c>
-      <c r="AK12" s="7" t="s">
+      <c r="AK12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AL12" s="8">
+      <c r="AL12" s="4">
         <v>0.001</v>
       </c>
-      <c r="AM12" s="7" t="s">
+      <c r="AM12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="AN12" s="8">
+      <c r="AN12" s="4">
         <v>0</v>
       </c>
     </row>
@@ -6133,22 +6214,22 @@
       <c r="AF13" s="4">
         <v>2.476</v>
       </c>
-      <c r="AI13" s="7" t="s">
+      <c r="AI13" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AJ13" s="8">
+      <c r="AJ13" s="4">
         <v>0.082</v>
       </c>
-      <c r="AK13" s="7" t="s">
+      <c r="AK13" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AL13" s="8">
+      <c r="AL13" s="4">
         <v>0.06</v>
       </c>
-      <c r="AM13" s="7" t="s">
+      <c r="AM13" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="AN13" s="8">
+      <c r="AN13" s="4">
         <v>0.025</v>
       </c>
     </row>
@@ -6161,10 +6242,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AD13"/>
+  <dimension ref="A1:AK13"/>
   <sheetViews>
     <sheetView topLeftCell="T7" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2:Z13"/>
+      <selection activeCell="AK2" sqref="AK2:AK13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.4444444444444" defaultRowHeight="15"/>
@@ -6172,7 +6253,7 @@
     <col min="1" max="16384" width="11.4444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" spans="1:30">
+    <row r="1" ht="18.75" spans="1:37">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -6263,8 +6344,26 @@
       <c r="AD1" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" ht="90.75" spans="1:30">
+      <c r="AF1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" ht="90.75" spans="1:37">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -6355,8 +6454,26 @@
       <c r="AD2" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" ht="54.75" spans="1:30">
+      <c r="AF2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK2" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" ht="54.75" spans="1:37">
       <c r="A3" s="3" t="s">
         <v>46</v>
       </c>
@@ -6447,8 +6564,26 @@
       <c r="AD3" s="4" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" ht="54.75" spans="1:30">
+      <c r="AF3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK3" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" ht="54.75" spans="1:37">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -6539,8 +6674,26 @@
       <c r="AD4" s="5">
         <v>2764800</v>
       </c>
-    </row>
-    <row r="5" ht="72.75" spans="1:30">
+      <c r="AF4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AG4" s="9">
+        <v>1440000</v>
+      </c>
+      <c r="AH4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI4" s="9">
+        <v>921600</v>
+      </c>
+      <c r="AJ4" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK4" s="9">
+        <v>230400</v>
+      </c>
+    </row>
+    <row r="5" ht="72.75" spans="1:37">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -6631,8 +6784,26 @@
       <c r="AD5" s="5">
         <v>3686472</v>
       </c>
-    </row>
-    <row r="6" ht="54.75" spans="1:30">
+      <c r="AF5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG5" s="9">
+        <v>1920072</v>
+      </c>
+      <c r="AH5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI5" s="9">
+        <v>1228872</v>
+      </c>
+      <c r="AJ5" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK5" s="9">
+        <v>307272</v>
+      </c>
+    </row>
+    <row r="6" ht="54.75" spans="1:37">
       <c r="A6" s="3" t="s">
         <v>49</v>
       </c>
@@ -6723,8 +6894,26 @@
       <c r="AD6" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" ht="144.75" spans="1:30">
+      <c r="AF6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG6" s="8">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI6" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" ht="144.75" spans="1:37">
       <c r="A7" s="3" t="s">
         <v>50</v>
       </c>
@@ -6815,8 +7004,26 @@
       <c r="AD7" s="4" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="8" ht="162.75" spans="1:30">
+      <c r="AF7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AG7" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI7" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ7" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AK7" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" ht="162.75" spans="1:37">
       <c r="A8" s="3" t="s">
         <v>70</v>
       </c>
@@ -6907,8 +7114,26 @@
       <c r="AD8" s="4" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" ht="36.75" spans="1:30">
+      <c r="AF8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG8" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AH8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="AJ8" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AK8" s="8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" ht="36.75" spans="1:37">
       <c r="A9" s="3" t="s">
         <v>90</v>
       </c>
@@ -6999,8 +7224,26 @@
       <c r="AD9" s="4">
         <v>0.516</v>
       </c>
-    </row>
-    <row r="10" ht="54.75" spans="1:30">
+      <c r="AF9" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="AG9" s="8">
+        <v>0.265</v>
+      </c>
+      <c r="AH9" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI9" s="8">
+        <v>0.161</v>
+      </c>
+      <c r="AJ9" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK9" s="8">
+        <v>0.059</v>
+      </c>
+    </row>
+    <row r="10" ht="54.75" spans="1:37">
       <c r="A10" s="3" t="s">
         <v>91</v>
       </c>
@@ -7091,8 +7334,26 @@
       <c r="AD10" s="4">
         <v>0.036</v>
       </c>
-    </row>
-    <row r="11" ht="36.75" spans="1:30">
+      <c r="AF10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AG10" s="8">
+        <v>0.015</v>
+      </c>
+      <c r="AH10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AI10" s="8">
+        <v>0.012</v>
+      </c>
+      <c r="AJ10" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK10" s="8">
+        <v>0.003</v>
+      </c>
+    </row>
+    <row r="11" ht="36.75" spans="1:37">
       <c r="A11" s="3" t="s">
         <v>92</v>
       </c>
@@ -7183,8 +7444,26 @@
       <c r="AD11" s="4">
         <v>62.568</v>
       </c>
-    </row>
-    <row r="12" ht="72.75" spans="1:30">
+      <c r="AF11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AG11" s="8">
+        <v>0.453</v>
+      </c>
+      <c r="AH11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AI11" s="8">
+        <v>0.257</v>
+      </c>
+      <c r="AJ11" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="AK11" s="8">
+        <v>0.298</v>
+      </c>
+    </row>
+    <row r="12" ht="72.75" spans="1:37">
       <c r="A12" s="3" t="s">
         <v>93</v>
       </c>
@@ -7275,8 +7554,26 @@
       <c r="AD12" s="4">
         <v>0.005</v>
       </c>
-    </row>
-    <row r="13" ht="54.75" spans="1:30">
+      <c r="AF12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG12" s="8">
+        <v>0.006</v>
+      </c>
+      <c r="AH12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI12" s="8">
+        <v>0.004</v>
+      </c>
+      <c r="AJ12" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK12" s="8">
+        <v>0.001</v>
+      </c>
+    </row>
+    <row r="13" ht="54.75" spans="1:37">
       <c r="A13" s="3" t="s">
         <v>94</v>
       </c>
@@ -7366,6 +7663,24 @@
       </c>
       <c r="AD13" s="4">
         <v>63.125</v>
+      </c>
+      <c r="AF13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AG13" s="8">
+        <v>0.739</v>
+      </c>
+      <c r="AH13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AI13" s="8">
+        <v>0.434</v>
+      </c>
+      <c r="AJ13" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK13" s="8">
+        <v>0.361</v>
       </c>
     </row>
   </sheetData>
@@ -7377,13 +7692,13 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A3:D6"/>
+  <dimension ref="A3:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15" outlineLevelCol="3"/>
   <sheetData>
     <row r="3" spans="3:4">
       <c r="C3" t="s">
@@ -7431,9 +7746,56 @@
         <v>0.45</v>
       </c>
     </row>
+    <row r="10" spans="3:4">
+      <c r="C10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11">
+        <v>0.099</v>
+      </c>
+      <c r="D11">
+        <v>0.487</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12">
+        <v>0.094</v>
+      </c>
+      <c r="D12">
+        <v>0.481</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13">
+        <v>0.072</v>
+      </c>
+      <c r="D13">
+        <v>0.471</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A4:A6"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>